<commit_message>
ManualSolve linked stack fix + start ResizableArray ManualSolve
</commit_message>
<xml_diff>
--- a/ManualSolve.xlsx
+++ b/ManualSolve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\Repo\Java\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Desktop\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0498A3D7-FB08-4769-A9C5-716286CAFE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9675719-155A-4A19-A672-35C5DF23E047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="6270" windowWidth="21525" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="0" windowWidth="25695" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>a*b / (c-a) + d *e</t>
   </si>
@@ -109,9 +109,6 @@
     <t>ab*ca-/de*+</t>
   </si>
   <si>
-    <t>+ *</t>
-  </si>
-  <si>
     <t>/ ( -</t>
   </si>
   <si>
@@ -119,19 +116,61 @@
   </si>
   <si>
     <t>Leonardo Davalos</t>
+  </si>
+  <si>
+    <t>a=2</t>
+  </si>
+  <si>
+    <t>b=3</t>
+  </si>
+  <si>
+    <t>c=4</t>
+  </si>
+  <si>
+    <t>d=5</t>
+  </si>
+  <si>
+    <t>e=6</t>
+  </si>
+  <si>
+    <t>↓</t>
+  </si>
+  <si>
+    <t>↑</t>
+  </si>
+  <si>
+    <t>*3</t>
+  </si>
+  <si>
+    <t>ab*ca-/de*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*+ </t>
+  </si>
+  <si>
+    <t>2*3</t>
+  </si>
+  <si>
+    <t>Dean Mah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,9 +193,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,184 +484,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>27</v>
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added GitHub repo link to ManualSolve excel
</commit_message>
<xml_diff>
--- a/ManualSolve.xlsx
+++ b/ManualSolve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Desktop\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BC0122-E3B6-495D-8834-C8115F9CDE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729A861-71B5-44D4-91C9-E8E1FE9E25E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="0" windowWidth="38190" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>a*b / (c-a) + d *e</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>3+30</t>
+  </si>
+  <si>
+    <t>GitHub repo Link</t>
+  </si>
+  <si>
+    <t>https://github.com/CS-2400-Team-DL/Project2.git</t>
+  </si>
+  <si>
+    <t>Task 4</t>
+  </si>
+  <si>
+    <t>Task 1</t>
   </si>
 </sst>
 </file>
@@ -202,7 +214,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,11 +222,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,7 +252,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -508,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AK27"/>
+  <dimension ref="B1:AK28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK25" sqref="AK25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +557,11 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -696,134 +734,137 @@
       </c>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="G20" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="D23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N23" s="1">
+      <c r="N23" s="4">
         <v>-2</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O23" s="4">
         <v>-2</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="P23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="R23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="S23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T23" s="1" t="s">
+      <c r="T23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="U23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="4" t="s">
+      <c r="V23" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="W23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="X23" s="1" t="s">
+      <c r="X23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y23" s="1" t="s">
+      <c r="Y23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Z23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB23" s="1" t="s">
+      <c r="Z23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AC23" s="1" t="s">
+      <c r="AC23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AD23" s="1" t="s">
+      <c r="AD23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AE23" s="1" t="s">
+      <c r="AE23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AF23" s="1" t="s">
+      <c r="AF23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AG23" s="1" t="s">
+      <c r="AG23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH23" s="2" t="s">
+      <c r="AH23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AI23" s="2" t="s">
+      <c r="AI23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AJ23" s="1" t="s">
+      <c r="AJ23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AK23" s="1" t="s">
+      <c r="AK23" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1080,6 +1121,14 @@
       </c>
       <c r="AA27" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>